<commit_message>
Add horizontal alignment "fill" to cell
</commit_message>
<xml_diff>
--- a/Excel.TemplateEngine.Tests/FileGeneratingTests/Files/template.xlsx
+++ b/Excel.TemplateEngine.Tests/FileGeneratingTests/Files/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="170" windowWidth="14810" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Покупатель:</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Template:RootTemplate:A1:A4</t>
+  </si>
+  <si>
+    <t>1232618020901658,2618020901658,2618020901658</t>
   </si>
 </sst>
 </file>
@@ -54,12 +57,20 @@
     <numFmt numFmtId="164" formatCode="#,##0.00&quot;р.&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -153,27 +164,30 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -488,24 +502,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40.54296875" customWidth="1"/>
+    <col min="2" max="2" width="34.26953125" customWidth="1"/>
+    <col min="3" max="3" width="34.81640625" customWidth="1"/>
+    <col min="4" max="4" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="8">
         <v>123.45</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="14" t="s">
+        <v>10</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -514,13 +528,13 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2"/>
@@ -530,10 +544,10 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
@@ -546,7 +560,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -557,7 +571,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="4"/>
       <c r="C7" s="1"/>
@@ -568,12 +582,12 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
         <v>0</v>
@@ -588,7 +602,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="5" t="s">
         <v>2</v>
@@ -605,7 +619,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -616,75 +630,75 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>

</xml_diff>